<commit_message>
citas creadas semana 26 feb
</commit_message>
<xml_diff>
--- a/datos/citas_creadas.xlsx
+++ b/datos/citas_creadas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Repositorios\estadistica_agendamientos\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB7A1A4-524E-47B5-8DBD-95B40E824310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB60E5F-52F5-41DF-A108-34C4723B4DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,18 +371,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,8 +396,11 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="2">
+        <v>45354</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -408,8 +413,11 @@
       <c r="D2">
         <v>1245</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -422,8 +430,11 @@
       <c r="D3">
         <v>1281</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -436,8 +447,11 @@
       <c r="D4">
         <v>1275</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -450,8 +464,11 @@
       <c r="D5">
         <v>3015</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>3054</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -463,6 +480,9 @@
       </c>
       <c r="D6">
         <v>83</v>
+      </c>
+      <c r="E6">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>